<commit_message>
processing column exp samples
</commit_message>
<xml_diff>
--- a/Laboratory_Processing_Metadata_Files/Column_exp_sample_list.xlsx
+++ b/Laboratory_Processing_Metadata_Files/Column_exp_sample_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest_ionic_strength/Laboratory_Processing_Metadata_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7535C8-AF28-F345-888D-D819F814679C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53632FCE-E4AB-6D46-883B-B9E09A988E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1120" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{5A739749-27BB-B242-A186-59495B9E7D37}"/>
+    <workbookView xWindow="1740" yWindow="-19600" windowWidth="28040" windowHeight="17440" xr2:uid="{5A739749-27BB-B242-A186-59495B9E7D37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="319">
   <si>
     <t>Random_ID</t>
   </si>
@@ -987,6 +987,15 @@
   </si>
   <si>
     <t>Sample_Name</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Sample wt</t>
+  </si>
+  <si>
+    <t>Total vol</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA188182-B9D1-EB45-B881-C3536C10ABB3}">
   <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2497,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A07F62-F963-7149-84E2-F1E5D29E8C9A}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2509,15 +2518,27 @@
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>289</v>
       </c>
       <c r="B1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>272</v>
       </c>
@@ -2525,7 +2546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>273</v>
       </c>
@@ -2533,7 +2554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>274</v>
       </c>
@@ -2541,7 +2562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>275</v>
       </c>
@@ -2549,7 +2570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>276</v>
       </c>
@@ -2557,7 +2578,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>277</v>
       </c>
@@ -2565,7 +2586,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>278</v>
       </c>
@@ -2573,7 +2594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -2581,7 +2602,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2589,7 +2610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2597,7 +2618,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2605,7 +2626,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2613,7 +2634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2621,7 +2642,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2629,7 +2650,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3125,10 +3146,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A25B3E-B363-AE46-961B-30B5A2C263E1}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3137,15 +3158,27 @@
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>289</v>
       </c>
       <c r="B1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>272</v>
       </c>
@@ -3153,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>273</v>
       </c>
@@ -3161,7 +3194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>274</v>
       </c>
@@ -3169,7 +3202,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>275</v>
       </c>
@@ -3177,7 +3210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -3185,7 +3218,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>311</v>
       </c>
@@ -3193,7 +3226,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>278</v>
       </c>
@@ -3201,7 +3234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>303</v>
       </c>
@@ -3209,7 +3242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>292</v>
       </c>
@@ -3217,7 +3250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>293</v>
       </c>
@@ -3225,7 +3258,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -3233,7 +3266,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>309</v>
       </c>
@@ -3241,7 +3274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>295</v>
       </c>
@@ -3249,7 +3282,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -3257,7 +3290,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>297</v>
       </c>
@@ -3753,10 +3786,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B4DCF3-16CC-6E40-84B3-FD498D5C88FF}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3765,15 +3798,27 @@
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>315</v>
       </c>
       <c r="B1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>272</v>
       </c>
@@ -3781,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>273</v>
       </c>
@@ -3789,7 +3834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>274</v>
       </c>
@@ -3797,7 +3842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>275</v>
       </c>
@@ -3805,7 +3850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>314</v>
       </c>
@@ -3813,7 +3858,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>311</v>
       </c>
@@ -3821,7 +3866,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>278</v>
       </c>
@@ -3829,7 +3874,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>303</v>
       </c>
@@ -3837,7 +3882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -3845,7 +3890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -3853,7 +3898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -3861,7 +3906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -3869,7 +3914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3877,7 +3922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -3885,7 +3930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>86</v>
       </c>

</xml_diff>